<commit_message>
Adds whole-year contribution & growth projection
</commit_message>
<xml_diff>
--- a/Rachel_money.xlsx
+++ b/Rachel_money.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\AF Finance Projector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C223E60B-54A3-455B-BD7F-D3979340E6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E30C509-CED7-487D-BF15-9AD989420E97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11952" yWindow="372" windowWidth="17868" windowHeight="10926" activeTab="2" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
+    <workbookView xWindow="2460" yWindow="246" windowWidth="17868" windowHeight="10926" activeTab="1" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Career Stats" sheetId="3" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
-  <si>
-    <t>Account Balance</t>
-  </si>
-  <si>
-    <t>Earning estimate (annual percent)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>TSP</t>
   </si>
@@ -48,9 +42,6 @@
     <t>Roth IRA</t>
   </si>
   <si>
-    <t>USAA</t>
-  </si>
-  <si>
     <t>Savings</t>
   </si>
   <si>
@@ -132,13 +123,28 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Account Name/Type (TSP and IRA handled differently)</t>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Growth Percent</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Checking</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -182,10 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,9 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9998D99-70A6-4C06-AF0F-49F1CC8DE041}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -514,23 +519,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>42879</v>
@@ -538,7 +543,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>78251</v>
@@ -546,23 +551,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>1000</v>
@@ -570,7 +575,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>40000</v>
@@ -578,7 +583,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -586,10 +591,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -603,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD186C03-94C1-42B8-B1CE-933D932337AA}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -615,27 +620,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1000</v>
@@ -646,10 +651,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>1200</v>
@@ -660,10 +665,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>900</v>
@@ -674,10 +679,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>400</v>
@@ -695,76 +700,92 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284EEA50-EF27-48FB-84ED-BA5F838EB730}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.5234375" customWidth="1"/>
-    <col min="2" max="2" width="14.9453125" customWidth="1"/>
-    <col min="3" max="3" width="14.62890625" customWidth="1"/>
+    <col min="1" max="1" width="6.68359375" customWidth="1"/>
+    <col min="2" max="2" width="9.578125" customWidth="1"/>
+    <col min="3" max="3" width="10.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="C3" s="3">
+        <v>15000</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>10000</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>15000</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="C4" s="3">
+        <v>7500</v>
+      </c>
+      <c r="D4">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3">
         <v>5000</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>7500</v>
-      </c>
-      <c r="C5">
-        <v>1.45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -784,13 +805,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds monthly contribution/growth in boring years
</commit_message>
<xml_diff>
--- a/Rachel_money.xlsx
+++ b/Rachel_money.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\AF Finance Projector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E30C509-CED7-487D-BF15-9AD989420E97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B64C3BF-8CBA-42EE-8DB2-FDD564847C76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="246" windowWidth="17868" windowHeight="10926" activeTab="1" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
+    <workbookView xWindow="7254" yWindow="354" windowWidth="17868" windowHeight="10926" activeTab="1" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Career Stats" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>TSP</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Cost of Living</t>
   </si>
   <si>
-    <t>Cost of Living (Leave blank for constant)</t>
-  </si>
-  <si>
     <t>State Tax</t>
   </si>
   <si>
@@ -136,6 +133,18 @@
   </si>
   <si>
     <t>Checking</t>
+  </si>
+  <si>
+    <t>State Taxes</t>
+  </si>
+  <si>
+    <t>Dependents</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Move Month</t>
   </si>
 </sst>
 </file>
@@ -583,7 +592,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -591,10 +600,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -606,19 +615,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD186C03-94C1-42B8-B1CE-933D932337AA}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="11.62890625" customWidth="1"/>
     <col min="3" max="3" width="11.578125" customWidth="1"/>
+    <col min="7" max="7" width="11.05078125" customWidth="1"/>
+    <col min="8" max="8" width="10.3671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -632,12 +643,24 @@
         <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -649,7 +672,7 @@
         <v>78251</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2023</v>
       </c>
@@ -663,7 +686,7 @@
         <v>78251</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2024</v>
       </c>
@@ -677,7 +700,7 @@
         <v>78251</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2025</v>
       </c>
@@ -715,16 +738,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -774,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3">
         <v>5000</v>

</xml_diff>

<commit_message>
working through projections changes
</commit_message>
<xml_diff>
--- a/Rachel_money.xlsx
+++ b/Rachel_money.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\AF Finance Projector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B64C3BF-8CBA-42EE-8DB2-FDD564847C76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37D8028-1B04-4E0E-A387-183600C91AF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7254" yWindow="354" windowWidth="17868" windowHeight="10926" activeTab="1" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
+    <workbookView xWindow="10812" yWindow="192" windowWidth="11952" windowHeight="10926" activeTab="1" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Career Stats" sheetId="3" r:id="rId1"/>
     <sheet name="Career Projection" sheetId="4" r:id="rId2"/>
-    <sheet name="Assets" sheetId="1" r:id="rId3"/>
-    <sheet name="Debts" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Assets" sheetId="1" r:id="rId4"/>
+    <sheet name="Debts" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>TSP</t>
   </si>
@@ -84,30 +85,15 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Additional Income</t>
   </si>
   <si>
-    <t>Highest Rank (or date of separation)</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
     <t>O-3</t>
   </si>
   <si>
     <t>O-4</t>
   </si>
   <si>
-    <t>O-5</t>
-  </si>
-  <si>
-    <t>O-6</t>
-  </si>
-  <si>
     <t>Cost of Living</t>
   </si>
   <si>
@@ -138,13 +124,25 @@
     <t>State Taxes</t>
   </si>
   <si>
-    <t>Dependents</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>Move Month</t>
+    <t>Promote</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Move Date</t>
+  </si>
+  <si>
+    <t>Promote Date</t>
+  </si>
+  <si>
+    <t>Other Date</t>
+  </si>
+  <si>
+    <t>Anniversary</t>
+  </si>
+  <si>
+    <t>Kid Birth Date</t>
   </si>
 </sst>
 </file>
@@ -185,10 +183,39 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -197,11 +224,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9998D99-70A6-4C06-AF0F-49F1CC8DE041}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -555,7 +593,7 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>78251</v>
+        <v>39540</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -584,7 +622,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>40000</v>
@@ -592,7 +630,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -600,10 +638,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -615,104 +653,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD186C03-94C1-42B8-B1CE-933D932337AA}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="9.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.62890625" customWidth="1"/>
-    <col min="3" max="3" width="11.578125" customWidth="1"/>
-    <col min="7" max="7" width="11.05078125" customWidth="1"/>
-    <col min="8" max="8" width="10.3671875" customWidth="1"/>
+    <col min="3" max="3" width="9.41796875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.1015625" customWidth="1"/>
+    <col min="6" max="6" width="13.05078125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="10.3671875" customWidth="1"/>
+    <col min="8" max="8" width="12.734375" customWidth="1"/>
+    <col min="9" max="9" width="10.5234375" customWidth="1"/>
+    <col min="10" max="10" width="16.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>2020</v>
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
+        <v>44341</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-      <c r="D2">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8">
+        <v>43881</v>
+      </c>
+      <c r="D2" s="7">
         <v>78251</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>2023</v>
+      <c r="E2" s="1">
+        <v>44456</v>
+      </c>
+      <c r="F2" s="11">
+        <v>45091</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44999</v>
+      </c>
+      <c r="H2" s="9">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
+        <v>46532</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3">
-        <v>1200</v>
-      </c>
-      <c r="D3">
-        <v>78251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>2024</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>900</v>
-      </c>
-      <c r="D4">
-        <v>78251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>2025</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>400</v>
-      </c>
-      <c r="D5">
-        <v>78251</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C3" s="8">
+        <v>46438</v>
+      </c>
+      <c r="D3" s="7">
+        <v>80841</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45398</v>
+      </c>
+      <c r="J3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="1">
+        <v>44364</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="5"/>
+      <c r="D14" s="7"/>
+      <c r="F14" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -722,11 +788,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D3A119-5C9C-4417-B974-5C8926016B51}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284EEA50-EF27-48FB-84ED-BA5F838EB730}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -738,16 +816,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -797,7 +875,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3">
         <v>5000</v>
@@ -812,7 +890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163A2BBC-ED5C-49F5-B3CD-41E2B3A7419C}">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Pulls career projections from spreadsheet and updates member. No account updates yet.
</commit_message>
<xml_diff>
--- a/Rachel_money.xlsx
+++ b/Rachel_money.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\AF Finance Projector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37D8028-1B04-4E0E-A387-183600C91AF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3358C3B-4421-45AE-B189-73A0EDDFA6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10812" yWindow="192" windowWidth="11952" windowHeight="10926" activeTab="1" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
   </bookViews>
@@ -124,12 +124,6 @@
     <t>State Taxes</t>
   </si>
   <si>
-    <t>Promote</t>
-  </si>
-  <si>
-    <t>Move</t>
-  </si>
-  <si>
     <t>Move Date</t>
   </si>
   <si>
@@ -143,6 +137,12 @@
   </si>
   <si>
     <t>Kid Birth Date</t>
+  </si>
+  <si>
+    <t>New Zip</t>
+  </si>
+  <si>
+    <t>New Rank</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -675,25 +675,25 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Adds field in career stats to bound prediction
</commit_message>
<xml_diff>
--- a/Rachel_money.xlsx
+++ b/Rachel_money.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\AF Finance Projector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3358C3B-4421-45AE-B189-73A0EDDFA6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331E8E5D-C2DF-4AD0-996A-913A15836036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10812" yWindow="192" windowWidth="11952" windowHeight="10926" activeTab="1" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
+    <workbookView xWindow="1062" yWindow="1398" windowWidth="16056" windowHeight="10926" xr2:uid="{1A0F8964-9FB7-4D3B-818B-2A72975BD45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Career Stats" sheetId="3" r:id="rId1"/>
     <sheet name="Career Projection" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Assets" sheetId="1" r:id="rId4"/>
-    <sheet name="Debts" sheetId="2" r:id="rId5"/>
+    <sheet name="Assets" sheetId="1" r:id="rId3"/>
+    <sheet name="Debts" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>TSP</t>
   </si>
@@ -143,6 +142,15 @@
   </si>
   <si>
     <t>New Rank</t>
+  </si>
+  <si>
+    <t>Brokerage</t>
+  </si>
+  <si>
+    <t>O-5</t>
+  </si>
+  <si>
+    <t>Project Through</t>
   </si>
 </sst>
 </file>
@@ -224,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -234,10 +242,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9998D99-70A6-4C06-AF0F-49F1CC8DE041}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -617,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -625,7 +634,7 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>40000</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -642,6 +651,14 @@
       </c>
       <c r="B10" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <v>2033</v>
       </c>
     </row>
   </sheetData>
@@ -655,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD186C03-94C1-42B8-B1CE-933D932337AA}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -666,7 +683,7 @@
     <col min="3" max="3" width="9.41796875" style="5" customWidth="1"/>
     <col min="4" max="4" width="11.578125" style="7" customWidth="1"/>
     <col min="5" max="5" width="12.1015625" customWidth="1"/>
-    <col min="6" max="6" width="13.05078125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.05078125" style="11" customWidth="1"/>
     <col min="7" max="7" width="10.3671875" customWidth="1"/>
     <col min="8" max="8" width="12.734375" customWidth="1"/>
     <col min="9" max="9" width="10.5234375" customWidth="1"/>
@@ -689,7 +706,7 @@
       <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -713,22 +730,18 @@
         <v>17</v>
       </c>
       <c r="C2" s="8">
-        <v>43881</v>
+        <v>43852</v>
       </c>
       <c r="D2" s="7">
         <v>78251</v>
       </c>
-      <c r="E2" s="1">
-        <v>44456</v>
-      </c>
-      <c r="F2" s="11">
-        <v>45091</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="1">
-        <v>44999</v>
-      </c>
-      <c r="H2" s="9">
-        <v>45000</v>
+        <v>45060</v>
+      </c>
+      <c r="H2" s="12">
+        <v>43000</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -739,24 +752,58 @@
         <v>18</v>
       </c>
       <c r="C3" s="8">
-        <v>46438</v>
+        <v>45060</v>
       </c>
       <c r="D3" s="7">
+        <v>20755</v>
+      </c>
+      <c r="G3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="J3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <v>47993</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="8">
+        <v>46138</v>
+      </c>
+      <c r="D4" s="7">
         <v>80841</v>
       </c>
-      <c r="G3" s="1">
-        <v>45398</v>
-      </c>
-      <c r="J3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="G4" s="1">
-        <v>44364</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
+        <v>46138</v>
+      </c>
+      <c r="H4" s="3">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" s="8">
+        <v>47279</v>
+      </c>
+      <c r="D5" s="7">
+        <v>78251</v>
+      </c>
+      <c r="G5" s="1">
+        <v>47289</v>
+      </c>
+      <c r="H5" s="13">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="1">
+        <v>44197</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -765,7 +812,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="6"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
@@ -778,7 +825,7 @@
     <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="5"/>
       <c r="D14" s="7"/>
-      <c r="F14" s="12"/>
+      <c r="F14" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -788,23 +835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D3A119-5C9C-4417-B974-5C8926016B51}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284EEA50-EF27-48FB-84ED-BA5F838EB730}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -850,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>15000</v>
+        <v>4000</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -861,13 +896,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3">
-        <v>7500</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1.45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -875,12 +910,26 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <v>5000</v>
       </c>
       <c r="D5">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4000</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
     </row>
@@ -890,28 +939,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163A2BBC-ED5C-49F5-B3CD-41E2B3A7419C}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.7890625" customWidth="1"/>
     <col min="2" max="2" width="15.1015625" customWidth="1"/>
+    <col min="3" max="3" width="13.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>